<commit_message>
Import and assignment (initial)
</commit_message>
<xml_diff>
--- a/WorkshopAssignmentApp/wwwroot/Workshop-Excel-Template.xlsx
+++ b/WorkshopAssignmentApp/wwwroot/Workshop-Excel-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6997db4dc8217659/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\youth-meetings-workshop-assignment\WorkshopAssignmentApp\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{F1B00E92-36DD-45FD-BC42-DCA1C1D6B7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50ECB176-350B-4D7A-9A36-E4CF16B8039E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7D45FD-CF48-4967-9697-DDD2B93A2507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30840" yWindow="1170" windowWidth="24990" windowHeight="13560" activeTab="1" xr2:uid="{1BDAB623-5FF0-44E2-B9C7-157E55438AF7}"/>
+    <workbookView xWindow="2370" yWindow="2242" windowWidth="18105" windowHeight="12781" activeTab="1" xr2:uid="{1BDAB623-5FF0-44E2-B9C7-157E55438AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Konfiguration" sheetId="1" r:id="rId1"/>
@@ -149,11 +149,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C0A3F44E-FBDA-4B91-8323-18C14BFAE2A5}" name="Table6" displayName="Table6" ref="A1:G80" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C0A3F44E-FBDA-4B91-8323-18C14BFAE2A5}" name="Participants" displayName="Participants" ref="A1:G80" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:G80" xr:uid="{4D56E9C7-D954-4812-98C4-CBC8EFC9496E}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E0582282-B120-4267-A232-7B210FEBA6A9}" name="Person"/>
@@ -518,14 +518,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.265625" customWidth="1"/>
+    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -547,7 +547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -558,7 +558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -580,7 +580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -591,13 +591,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -605,7 +605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -621,7 +621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -647,19 +647,19 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.265625" customWidth="1"/>
+    <col min="2" max="4" width="9.73046875" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -672,22 +672,22 @@
       <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>

</xml_diff>